<commit_message>
Update produced and sent areas around Admin DB export. User CLI back in scope.
</commit_message>
<xml_diff>
--- a/risks.xlsx
+++ b/risks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="336">
   <si>
     <t>Severity</t>
   </si>
@@ -352,6 +352,15 @@
     <t>missing-hardening@host-cluster-kubernetes-api</t>
   </si>
   <si>
+    <t>User CLI</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at User CLI</t>
+  </si>
+  <si>
+    <t>missing-hardening@user-cli</t>
+  </si>
+  <si>
     <t>Missing Identity Provider Isolation</t>
   </si>
   <si>
@@ -475,6 +484,15 @@
     <t>server-side-request-forgery@api-server@repo-server@api-server&gt;fetching-rendered-manifests-from-cache</t>
   </si>
   <si>
+    <t>Export Database</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at API Server server-side web-requesting the target User CLI via Export Database</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@api-server@user-cli@api-server&gt;export-database</t>
+  </si>
+  <si>
     <t>Application Controller</t>
   </si>
   <si>
@@ -610,6 +628,12 @@
     <t>server-side-request-forgery@repo-server@rendered-manifests-cache@repo-server&gt;send-receive-cached-rendered-manifests</t>
   </si>
   <si>
+    <t>Server-Side Request Forgery (SSRF) risk at User CLI server-side web-requesting the target API Server via Make Requests to API Server</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@user-cli@api-server@user-cli&gt;make-requests-to-api-server</t>
+  </si>
+  <si>
     <t>CWE-501</t>
   </si>
   <si>
@@ -799,7 +823,7 @@
     <t>Missing Identity Store</t>
   </si>
   <si>
-    <t>Missing Identity Store in the threat model (referencing asset Argo CD Maintainer Git Client as an example)</t>
+    <t>Missing Identity Store in the threat model (referencing asset User CLI as an example)</t>
   </si>
   <si>
     <t>Identity Store</t>
@@ -808,7 +832,7 @@
     <t>Include an identity store in the model if the application has a login.</t>
   </si>
   <si>
-    <t>missing-identity-store@argo-cd-maintainer-git-client</t>
+    <t>missing-identity-store@user-cli</t>
   </si>
   <si>
     <t>Missing Network Segmentation</t>
@@ -829,6 +853,12 @@
     <t>missing-network-segmentation@applicationset-controller</t>
   </si>
   <si>
+    <t>Missing Network Segmentation to further encapsulate and protect User CLI against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>missing-network-segmentation@user-cli</t>
+  </si>
+  <si>
     <t>Business Side</t>
   </si>
   <si>
@@ -970,6 +1000,12 @@
     <t>unnecessary-data-transfer@argo-cd-container-image-tag@argo-cd-source-repo@argo-cd-maintainer-git-client</t>
   </si>
   <si>
+    <t>Unnecessary Data Transfer of Argo CD Database Export data at User CLI from/to API Server</t>
+  </si>
+  <si>
+    <t>unnecessary-data-transfer@argocd-db-export@user-cli@api-server</t>
+  </si>
+  <si>
     <t>Unnecessary Data Transfer of Argo CD GitHub Push Token data at Argo CD Source Repo (GitHub) from/to Argo CD Maintainer Git Client</t>
   </si>
   <si>
@@ -986,18 +1022,6 @@
   </si>
   <si>
     <t>unnecessary-data-transfer@user-provided-secret@api-server@user-cli</t>
-  </si>
-  <si>
-    <t>Unnecessary Data Asset</t>
-  </si>
-  <si>
-    <t>Unnecessary Data Asset named Argo CD Database Export</t>
-  </si>
-  <si>
-    <t>Try to avoid having data assets that are not required/used.</t>
-  </si>
-  <si>
-    <t>unnecessary-data-asset@argocd-db-export</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1724,7 @@
         <v>36</v>
       </c>
       <c r="J3" s="19">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>37</v>
@@ -1808,7 +1832,7 @@
         <v>43</v>
       </c>
       <c r="J5" s="19">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" s="20" t="s">
         <v>48</v>
@@ -1862,7 +1886,7 @@
         <v>55</v>
       </c>
       <c r="J6" s="19">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K6" s="20" t="s">
         <v>56</v>
@@ -1916,7 +1940,7 @@
         <v>61</v>
       </c>
       <c r="J7" s="19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>62</v>
@@ -1970,7 +1994,7 @@
         <v>61</v>
       </c>
       <c r="J8" s="19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>64</v>
@@ -2024,7 +2048,7 @@
         <v>61</v>
       </c>
       <c r="J9" s="19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>66</v>
@@ -2078,7 +2102,7 @@
         <v>61</v>
       </c>
       <c r="J10" s="19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="20" t="s">
         <v>68</v>
@@ -2186,7 +2210,7 @@
         <v>74</v>
       </c>
       <c r="J12" s="19">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K12" s="20" t="s">
         <v>75</v>
@@ -2240,7 +2264,7 @@
         <v>78</v>
       </c>
       <c r="J13" s="19">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K13" s="20" t="s">
         <v>79</v>
@@ -2294,7 +2318,7 @@
         <v>36</v>
       </c>
       <c r="J14" s="19">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>81</v>
@@ -2510,7 +2534,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="19">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K18" s="20" t="s">
         <v>99</v>
@@ -2618,7 +2642,7 @@
         <v>43</v>
       </c>
       <c r="J20" s="19">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K20" s="20" t="s">
         <v>110</v>
@@ -2648,46 +2672,46 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>43</v>
       </c>
       <c r="J21" s="19">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="K21" s="20" t="s">
         <v>113</v>
       </c>
       <c r="L21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="M21" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="M21" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="N21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21" s="21" t="s">
-        <v>116</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>34</v>
@@ -2702,46 +2726,46 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="19">
+        <v>35</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="M22" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="N22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J22" s="19">
-        <v>44</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="L22" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="M22" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="N22" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O22" s="21" t="s">
-        <v>124</v>
       </c>
       <c r="P22" s="11" t="s">
         <v>34</v>
@@ -2759,43 +2783,43 @@
         <v>21</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J23" s="19">
+        <v>42</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="L23" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="M23" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="5" t="s">
+      <c r="N23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="J23" s="19">
-        <v>100</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M23" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="N23" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O23" s="21" t="s">
-        <v>131</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>34</v>
@@ -2806,44 +2830,44 @@
       <c r="T23" s="17"/>
     </row>
     <row r="24">
-      <c r="A24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="A24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H24" s="7" t="s">
+      <c r="F24" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>132</v>
+      <c r="I24" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="J24" s="19">
         <v>100</v>
       </c>
       <c r="K24" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M24" s="23" t="s">
         <v>133</v>
-      </c>
-      <c r="L24" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M24" s="23" t="s">
-        <v>130</v>
       </c>
       <c r="N24" s="23" t="s">
         <v>32</v>
@@ -2870,16 +2894,16 @@
         <v>22</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>27</v>
@@ -2894,10 +2918,10 @@
         <v>136</v>
       </c>
       <c r="L25" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M25" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N25" s="23" t="s">
         <v>32</v>
@@ -2924,16 +2948,16 @@
         <v>22</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>27</v>
@@ -2948,10 +2972,10 @@
         <v>139</v>
       </c>
       <c r="L26" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M26" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N26" s="23" t="s">
         <v>32</v>
@@ -2978,16 +3002,16 @@
         <v>22</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>27</v>
@@ -3002,10 +3026,10 @@
         <v>142</v>
       </c>
       <c r="L27" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M27" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N27" s="23" t="s">
         <v>32</v>
@@ -3032,16 +3056,16 @@
         <v>22</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>27</v>
@@ -3056,10 +3080,10 @@
         <v>145</v>
       </c>
       <c r="L28" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M28" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N28" s="23" t="s">
         <v>32</v>
@@ -3086,40 +3110,40 @@
         <v>22</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="J29" s="19">
         <v>100</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L29" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N29" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O29" s="21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P29" s="11" t="s">
         <v>34</v>
@@ -3140,40 +3164,40 @@
         <v>22</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="J30" s="19">
         <v>100</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L30" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M30" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N30" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O30" s="21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="P30" s="11" t="s">
         <v>34</v>
@@ -3194,40 +3218,40 @@
         <v>22</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J31" s="19">
         <v>100</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L31" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M31" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N31" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O31" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="P31" s="11" t="s">
         <v>34</v>
@@ -3248,40 +3272,40 @@
         <v>22</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="I32" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="19">
+        <v>100</v>
+      </c>
+      <c r="K32" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="J32" s="19">
-        <v>43</v>
-      </c>
-      <c r="K32" s="20" t="s">
+      <c r="L32" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M32" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="21" t="s">
         <v>155</v>
-      </c>
-      <c r="L32" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M32" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="N32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O32" s="21" t="s">
-        <v>156</v>
       </c>
       <c r="P32" s="11" t="s">
         <v>34</v>
@@ -3302,40 +3326,40 @@
         <v>22</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J33" s="19">
+        <v>100</v>
+      </c>
+      <c r="K33" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J33" s="19">
-        <v>43</v>
-      </c>
-      <c r="K33" s="20" t="s">
+      <c r="L33" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O33" s="21" t="s">
         <v>158</v>
-      </c>
-      <c r="L33" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M33" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="N33" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O33" s="21" t="s">
-        <v>159</v>
       </c>
       <c r="P33" s="11" t="s">
         <v>34</v>
@@ -3356,40 +3380,40 @@
         <v>22</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
       <c r="J34" s="19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L34" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M34" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N34" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O34" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="P34" s="11" t="s">
         <v>34</v>
@@ -3410,40 +3434,40 @@
         <v>22</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="J35" s="19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L35" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M35" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N35" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O35" s="21" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="P35" s="11" t="s">
         <v>34</v>
@@ -3464,40 +3488,40 @@
         <v>22</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="J36" s="19">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L36" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M36" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N36" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O36" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P36" s="11" t="s">
         <v>34</v>
@@ -3518,34 +3542,34 @@
         <v>22</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="J37" s="19">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K37" s="20" t="s">
         <v>168</v>
       </c>
       <c r="L37" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M37" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N37" s="23" t="s">
         <v>32</v>
@@ -3572,40 +3596,40 @@
         <v>22</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="J38" s="19">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L38" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M38" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N38" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="P38" s="11" t="s">
         <v>34</v>
@@ -3626,34 +3650,34 @@
         <v>22</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>173</v>
       </c>
       <c r="J39" s="19">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="K39" s="20" t="s">
         <v>174</v>
       </c>
       <c r="L39" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M39" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N39" s="23" t="s">
         <v>32</v>
@@ -3680,34 +3704,34 @@
         <v>22</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J40" s="19">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="K40" s="20" t="s">
         <v>176</v>
       </c>
       <c r="L40" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M40" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N40" s="23" t="s">
         <v>32</v>
@@ -3734,40 +3758,40 @@
         <v>22</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J41" s="19">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K41" s="20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L41" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M41" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N41" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O41" s="21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P41" s="11" t="s">
         <v>34</v>
@@ -3788,40 +3812,40 @@
         <v>22</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I42" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J42" s="19">
+        <v>31</v>
+      </c>
+      <c r="K42" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="J42" s="19">
-        <v>9</v>
-      </c>
-      <c r="K42" s="20" t="s">
+      <c r="L42" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M42" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N42" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O42" s="21" t="s">
         <v>183</v>
-      </c>
-      <c r="L42" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M42" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="N42" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O42" s="21" t="s">
-        <v>184</v>
       </c>
       <c r="P42" s="11" t="s">
         <v>34</v>
@@ -3842,40 +3866,40 @@
         <v>22</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J43" s="19">
+        <v>31</v>
+      </c>
+      <c r="K43" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="J43" s="19">
-        <v>36</v>
-      </c>
-      <c r="K43" s="20" t="s">
+      <c r="L43" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M43" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N43" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O43" s="21" t="s">
         <v>186</v>
-      </c>
-      <c r="L43" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M43" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="N43" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O43" s="21" t="s">
-        <v>187</v>
       </c>
       <c r="P43" s="11" t="s">
         <v>34</v>
@@ -3896,34 +3920,34 @@
         <v>22</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>188</v>
       </c>
       <c r="J44" s="19">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="K44" s="20" t="s">
         <v>189</v>
       </c>
       <c r="L44" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M44" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N44" s="23" t="s">
         <v>32</v>
@@ -3950,34 +3974,34 @@
         <v>22</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>191</v>
       </c>
       <c r="J45" s="19">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="K45" s="20" t="s">
         <v>192</v>
       </c>
       <c r="L45" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M45" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N45" s="23" t="s">
         <v>32</v>
@@ -4004,40 +4028,40 @@
         <v>22</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>61</v>
+        <v>194</v>
       </c>
       <c r="J46" s="19">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L46" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M46" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N46" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="P46" s="11" t="s">
         <v>34</v>
@@ -4058,40 +4082,40 @@
         <v>22</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>78</v>
+        <v>197</v>
       </c>
       <c r="J47" s="19">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K47" s="20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L47" s="23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M47" s="23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="N47" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="P47" s="11" t="s">
         <v>34</v>
@@ -4102,50 +4126,50 @@
       <c r="T47" s="17"/>
     </row>
     <row r="48">
-      <c r="A48" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H48" s="5" t="s">
+      <c r="A48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J48" s="19">
+        <v>42</v>
+      </c>
+      <c r="K48" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J48" s="19">
-        <v>13</v>
-      </c>
-      <c r="K48" s="20" t="s">
+      <c r="L48" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M48" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N48" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O48" s="21" t="s">
         <v>201</v>
-      </c>
-      <c r="L48" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="M48" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="N48" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O48" s="21" t="s">
-        <v>204</v>
       </c>
       <c r="P48" s="11" t="s">
         <v>34</v>
@@ -4156,50 +4180,50 @@
       <c r="T48" s="17"/>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>71</v>
+      <c r="A49" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="J49" s="19">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="K49" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L49" s="23" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="M49" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N49" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O49" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="N49" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O49" s="21" t="s">
-        <v>206</v>
       </c>
       <c r="P49" s="11" t="s">
         <v>34</v>
@@ -4210,50 +4234,50 @@
       <c r="T49" s="17"/>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>178</v>
+      <c r="A50" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="J50" s="19">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="K50" s="20" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L50" s="23" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="M50" s="23" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
       <c r="N50" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P50" s="11" t="s">
         <v>34</v>
@@ -4264,50 +4288,50 @@
       <c r="T50" s="17"/>
     </row>
     <row r="51">
-      <c r="A51" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>43</v>
+      <c r="A51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="J51" s="19">
         <v>13</v>
       </c>
       <c r="K51" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="L51" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="M51" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="L51" s="23" t="s">
+      <c r="N51" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O51" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="M51" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="N51" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O51" s="21" t="s">
-        <v>214</v>
       </c>
       <c r="P51" s="11" t="s">
         <v>34</v>
@@ -4318,50 +4342,50 @@
       <c r="T51" s="17"/>
     </row>
     <row r="52">
-      <c r="A52" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="H52" s="7" t="s">
+      <c r="A52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I52" s="7" t="s">
-        <v>43</v>
+      <c r="I52" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="J52" s="19">
         <v>13</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L52" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M52" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N52" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P52" s="11" t="s">
         <v>34</v>
@@ -4372,50 +4396,50 @@
       <c r="T52" s="17"/>
     </row>
     <row r="53">
-      <c r="A53" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="G53" s="7" t="s">
+      <c r="A53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J53" s="19">
+        <v>33</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="L53" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="H53" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J53" s="19">
-        <v>34</v>
-      </c>
-      <c r="K53" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="L53" s="23" t="s">
-        <v>212</v>
-      </c>
       <c r="M53" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N53" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P53" s="11" t="s">
         <v>34</v>
@@ -4436,40 +4460,40 @@
         <v>39</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J54" s="19">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="K54" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="L54" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="M54" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="L54" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M54" s="23" t="s">
+      <c r="N54" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O54" s="21" t="s">
         <v>222</v>
-      </c>
-      <c r="N54" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O54" s="21" t="s">
-        <v>223</v>
       </c>
       <c r="P54" s="11" t="s">
         <v>34</v>
@@ -4490,19 +4514,19 @@
         <v>39</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>43</v>
@@ -4511,19 +4535,19 @@
         <v>13</v>
       </c>
       <c r="K55" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="L55" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="M55" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="N55" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O55" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="L55" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M55" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="N55" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O55" s="21" t="s">
-        <v>225</v>
       </c>
       <c r="P55" s="11" t="s">
         <v>34</v>
@@ -4544,40 +4568,40 @@
         <v>39</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J56" s="19">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="K56" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="L56" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="M56" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="N56" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O56" s="21" t="s">
         <v>226</v>
-      </c>
-      <c r="L56" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M56" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="N56" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O56" s="21" t="s">
-        <v>227</v>
       </c>
       <c r="P56" s="11" t="s">
         <v>34</v>
@@ -4604,34 +4628,34 @@
         <v>85</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>60</v>
+        <v>178</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J57" s="19">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K57" s="20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L57" s="23" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M57" s="23" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="N57" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O57" s="21" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="P57" s="11" t="s">
         <v>34</v>
@@ -4658,34 +4682,34 @@
         <v>85</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>27</v>
+        <v>208</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J58" s="19">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="K58" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L58" s="23" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="M58" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="N58" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O58" s="21" t="s">
         <v>233</v>
-      </c>
-      <c r="N58" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="O58" s="21" t="s">
-        <v>235</v>
       </c>
       <c r="P58" s="11" t="s">
         <v>34</v>
@@ -4712,34 +4736,34 @@
         <v>85</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>153</v>
+        <v>70</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J59" s="19">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="K59" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L59" s="23" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="M59" s="23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="N59" s="23" t="s">
-        <v>234</v>
+        <v>32</v>
       </c>
       <c r="O59" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P59" s="11" t="s">
         <v>34</v>
@@ -4766,34 +4790,34 @@
         <v>85</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>164</v>
+        <v>60</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J60" s="19">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="K60" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L60" s="23" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="M60" s="23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="N60" s="23" t="s">
-        <v>234</v>
+        <v>32</v>
       </c>
       <c r="O60" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P60" s="11" t="s">
         <v>34</v>
@@ -4820,34 +4844,34 @@
         <v>85</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>240</v>
+        <v>27</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J61" s="19">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="K61" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L61" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="M61" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="L61" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="M61" s="23" t="s">
-        <v>233</v>
-      </c>
       <c r="N61" s="23" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="O61" s="21" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="P61" s="11" t="s">
         <v>34</v>
@@ -4874,34 +4898,34 @@
         <v>85</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J62" s="19">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="K62" s="20" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L62" s="23" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="M62" s="23" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="N62" s="23" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="O62" s="21" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P62" s="11" t="s">
         <v>34</v>
@@ -4928,34 +4952,34 @@
         <v>85</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
       <c r="I63" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J63" s="19">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="K63" s="20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L63" s="23" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="M63" s="23" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="N63" s="23" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="O63" s="21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="P63" s="11" t="s">
         <v>34</v>
@@ -4982,13 +5006,13 @@
         <v>85</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>43</v>
@@ -4997,19 +5021,19 @@
         <v>26</v>
       </c>
       <c r="K64" s="20" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="L64" s="23" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="M64" s="23" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="N64" s="23" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="O64" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="P64" s="11" t="s">
         <v>34</v>
@@ -5036,34 +5060,34 @@
         <v>85</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J65" s="19">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="K65" s="20" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L65" s="23" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="M65" s="23" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="N65" s="23" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="O65" s="21" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P65" s="11" t="s">
         <v>34</v>
@@ -5090,34 +5114,34 @@
         <v>85</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J66" s="19">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="K66" s="20" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L66" s="23" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="M66" s="23" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="N66" s="23" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="O66" s="21" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="P66" s="11" t="s">
         <v>34</v>
@@ -5135,43 +5159,43 @@
         <v>83</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J67" s="19">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="K67" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="L67" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="M67" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="N67" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="O67" s="21" t="s">
         <v>256</v>
-      </c>
-      <c r="L67" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M67" s="23" t="s">
-        <v>257</v>
-      </c>
-      <c r="N67" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O67" s="21" t="s">
-        <v>258</v>
       </c>
       <c r="P67" s="11" t="s">
         <v>34</v>
@@ -5189,43 +5213,43 @@
         <v>83</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>181</v>
+        <v>257</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J68" s="19">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K68" s="20" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L68" s="23" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="M68" s="23" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="N68" s="23" t="s">
-        <v>32</v>
+        <v>242</v>
       </c>
       <c r="O68" s="21" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="P68" s="11" t="s">
         <v>34</v>
@@ -5243,43 +5267,43 @@
         <v>83</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>86</v>
+        <v>227</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J69" s="19">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="K69" s="20" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="L69" s="23" t="s">
-        <v>114</v>
+        <v>240</v>
       </c>
       <c r="M69" s="23" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="N69" s="23" t="s">
-        <v>32</v>
+        <v>242</v>
       </c>
       <c r="O69" s="21" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="P69" s="11" t="s">
         <v>34</v>
@@ -5300,40 +5324,40 @@
         <v>22</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J70" s="19">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K70" s="20" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="L70" s="23" t="s">
-        <v>114</v>
+        <v>220</v>
       </c>
       <c r="M70" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N70" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O70" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="P70" s="11" t="s">
         <v>34</v>
@@ -5354,40 +5378,40 @@
         <v>22</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E71" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J71" s="19">
+        <v>56</v>
+      </c>
+      <c r="K71" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="L71" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="M71" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="N71" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O71" s="21" t="s">
         <v>272</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J71" s="19">
-        <v>100</v>
-      </c>
-      <c r="K71" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="L71" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="M71" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="N71" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O71" s="21" t="s">
-        <v>277</v>
       </c>
       <c r="P71" s="11" t="s">
         <v>34</v>
@@ -5408,40 +5432,40 @@
         <v>22</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>278</v>
+        <v>86</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>280</v>
+        <v>27</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J72" s="19">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K72" s="20" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="L72" s="23" t="s">
-        <v>282</v>
+        <v>117</v>
       </c>
       <c r="M72" s="23" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="N72" s="23" t="s">
-        <v>284</v>
+        <v>32</v>
       </c>
       <c r="O72" s="21" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="P72" s="11" t="s">
         <v>34</v>
@@ -5462,7 +5486,7 @@
         <v>22</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>85</v>
@@ -5471,31 +5495,31 @@
         <v>86</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J73" s="19">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="K73" s="20" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="L73" s="23" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="M73" s="23" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="N73" s="23" t="s">
-        <v>290</v>
+        <v>32</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="P73" s="11" t="s">
         <v>34</v>
@@ -5516,7 +5540,7 @@
         <v>22</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>85</v>
@@ -5525,31 +5549,31 @@
         <v>86</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>240</v>
+        <v>112</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J74" s="19">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="K74" s="20" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="L74" s="23" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="M74" s="23" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="N74" s="23" t="s">
-        <v>290</v>
+        <v>32</v>
       </c>
       <c r="O74" s="21" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="P74" s="11" t="s">
         <v>34</v>
@@ -5570,40 +5594,40 @@
         <v>22</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>85</v>
+        <v>281</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>86</v>
+        <v>282</v>
       </c>
       <c r="G75" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J75" s="19">
+        <v>100</v>
+      </c>
+      <c r="K75" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="L75" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="M75" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="H75" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I75" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J75" s="19">
-        <v>69</v>
-      </c>
-      <c r="K75" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="L75" s="23" t="s">
-        <v>288</v>
-      </c>
-      <c r="M75" s="23" t="s">
-        <v>289</v>
-      </c>
       <c r="N75" s="23" t="s">
-        <v>290</v>
+        <v>32</v>
       </c>
       <c r="O75" s="21" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="P75" s="11" t="s">
         <v>34</v>
@@ -5624,40 +5648,40 @@
         <v>22</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>254</v>
+        <v>288</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>172</v>
+        <v>290</v>
       </c>
       <c r="I76" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J76" s="19">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K76" s="20" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="L76" s="23" t="s">
-        <v>212</v>
+        <v>292</v>
       </c>
       <c r="M76" s="23" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="N76" s="23" t="s">
-        <v>32</v>
+        <v>294</v>
       </c>
       <c r="O76" s="21" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="P76" s="11" t="s">
         <v>34</v>
@@ -5668,50 +5692,50 @@
       <c r="T76" s="17"/>
     </row>
     <row r="77">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J77" s="19">
+        <v>100</v>
+      </c>
+      <c r="K77" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="L77" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="M77" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="N77" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="B77" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F77" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="G77" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="H77" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J77" s="19">
-        <v>13</v>
-      </c>
-      <c r="K77" s="20" t="s">
+      <c r="O77" s="21" t="s">
         <v>301</v>
-      </c>
-      <c r="L77" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M77" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="N77" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O77" s="21" t="s">
-        <v>302</v>
       </c>
       <c r="P77" s="11" t="s">
         <v>34</v>
@@ -5722,50 +5746,50 @@
       <c r="T77" s="17"/>
     </row>
     <row r="78">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J78" s="19">
+        <v>26</v>
+      </c>
+      <c r="K78" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="L78" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="M78" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="N78" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="B78" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F78" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="G78" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="H78" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I78" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J78" s="19">
-        <v>13</v>
-      </c>
-      <c r="K78" s="20" t="s">
+      <c r="O78" s="21" t="s">
         <v>303</v>
-      </c>
-      <c r="L78" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M78" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="N78" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O78" s="21" t="s">
-        <v>304</v>
       </c>
       <c r="P78" s="11" t="s">
         <v>34</v>
@@ -5776,50 +5800,50 @@
       <c r="T78" s="17"/>
     </row>
     <row r="79">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J79" s="19">
+        <v>67</v>
+      </c>
+      <c r="K79" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="L79" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="M79" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="N79" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="B79" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F79" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="H79" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I79" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J79" s="19">
-        <v>34</v>
-      </c>
-      <c r="K79" s="20" t="s">
+      <c r="O79" s="21" t="s">
         <v>305</v>
-      </c>
-      <c r="L79" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M79" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="N79" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O79" s="21" t="s">
-        <v>306</v>
       </c>
       <c r="P79" s="11" t="s">
         <v>34</v>
@@ -5837,43 +5861,43 @@
         <v>83</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>249</v>
+        <v>178</v>
       </c>
       <c r="I80" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J80" s="19">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K80" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="L80" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="M80" s="23" t="s">
+        <v>308</v>
+      </c>
+      <c r="N80" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O80" s="21" t="s">
         <v>309</v>
-      </c>
-      <c r="L80" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="M80" s="23" t="s">
-        <v>311</v>
-      </c>
-      <c r="N80" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O80" s="21" t="s">
-        <v>312</v>
       </c>
       <c r="P80" s="11" t="s">
         <v>34</v>
@@ -5884,50 +5908,50 @@
       <c r="T80" s="17"/>
     </row>
     <row r="81">
-      <c r="A81" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E81" s="8" t="s">
+      <c r="A81" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E81" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F81" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="I81" s="7" t="s">
+      <c r="F81" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I81" s="9" t="s">
         <v>43</v>
       </c>
       <c r="J81" s="19">
         <v>13</v>
       </c>
       <c r="K81" s="20" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L81" s="23" t="s">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="M81" s="23" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N81" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O81" s="21" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="P81" s="11" t="s">
         <v>34</v>
@@ -5938,50 +5962,50 @@
       <c r="T81" s="17"/>
     </row>
     <row r="82">
-      <c r="A82" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E82" s="8" t="s">
+      <c r="A82" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="I82" s="7" t="s">
+      <c r="F82" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="H82" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I82" s="9" t="s">
         <v>43</v>
       </c>
       <c r="J82" s="19">
         <v>13</v>
       </c>
       <c r="K82" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L82" s="23" t="s">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="M82" s="23" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N82" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O82" s="21" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="P82" s="11" t="s">
         <v>34</v>
@@ -5992,50 +6016,50 @@
       <c r="T82" s="17"/>
     </row>
     <row r="83">
-      <c r="A83" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E83" s="8" t="s">
+      <c r="A83" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E83" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F83" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I83" s="7" t="s">
+      <c r="F83" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="H83" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I83" s="9" t="s">
         <v>43</v>
       </c>
       <c r="J83" s="19">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="K83" s="20" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="L83" s="23" t="s">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="M83" s="23" t="s">
+        <v>308</v>
+      </c>
+      <c r="N83" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O83" s="21" t="s">
         <v>316</v>
-      </c>
-      <c r="N83" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O83" s="21" t="s">
-        <v>321</v>
       </c>
       <c r="P83" s="11" t="s">
         <v>34</v>
@@ -6053,43 +6077,43 @@
         <v>83</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>86</v>
+        <v>317</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>27</v>
+        <v>257</v>
       </c>
       <c r="I84" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J84" s="19">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="K84" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="L84" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="M84" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="N84" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O84" s="21" t="s">
         <v>322</v>
-      </c>
-      <c r="L84" s="23" t="s">
-        <v>315</v>
-      </c>
-      <c r="M84" s="23" t="s">
-        <v>316</v>
-      </c>
-      <c r="N84" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O84" s="21" t="s">
-        <v>323</v>
       </c>
       <c r="P84" s="11" t="s">
         <v>34</v>
@@ -6100,41 +6124,41 @@
       <c r="T84" s="17"/>
     </row>
     <row r="85">
-      <c r="A85" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D85" s="10" t="s">
+      <c r="A85" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E85" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F85" s="10" t="s">
+      <c r="F85" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G85" s="9" t="s">
+      <c r="G85" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J85" s="19">
+        <v>13</v>
+      </c>
+      <c r="K85" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="H85" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J85" s="19">
-        <v>0</v>
-      </c>
-      <c r="K85" s="20" t="s">
+      <c r="L85" s="23" t="s">
         <v>325</v>
-      </c>
-      <c r="L85" s="23" t="s">
-        <v>315</v>
       </c>
       <c r="M85" s="23" t="s">
         <v>326</v>
@@ -6152,6 +6176,222 @@
       <c r="R85" s="18"/>
       <c r="S85" s="18"/>
       <c r="T85" s="17"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J86" s="19">
+        <v>56</v>
+      </c>
+      <c r="K86" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="L86" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="M86" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="N86" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O86" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="P86" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q86" s="20"/>
+      <c r="R86" s="18"/>
+      <c r="S86" s="18"/>
+      <c r="T86" s="17"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J87" s="19">
+        <v>13</v>
+      </c>
+      <c r="K87" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="L87" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="M87" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="N87" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O87" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="P87" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q87" s="20"/>
+      <c r="R87" s="18"/>
+      <c r="S87" s="18"/>
+      <c r="T87" s="17"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J88" s="19">
+        <v>67</v>
+      </c>
+      <c r="K88" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="L88" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="M88" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="N88" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O88" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="P88" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q88" s="20"/>
+      <c r="R88" s="18"/>
+      <c r="S88" s="18"/>
+      <c r="T88" s="17"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J89" s="19">
+        <v>100</v>
+      </c>
+      <c r="K89" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="L89" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="M89" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="N89" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O89" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="P89" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q89" s="20"/>
+      <c r="R89" s="18"/>
+      <c r="S89" s="18"/>
+      <c r="T89" s="17"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>